<commit_message>
MVsB5_BT_Audio_SDK_V0.8.0 - *.pdf *.ini *.html *.xlsx
</commit_message>
<xml_diff>
--- a/BT_Audio_APP/app_src/components/audio/effect_control/params_msg_mapping.xlsx
+++ b/BT_Audio_APP/app_src/components/audio/effect_control/params_msg_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\b5_sdk\BT_Audio_APP\app_src\components\audio\effect_control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\B5\B5_SDK_24Bit_V3_sync\BT_Audio_APP\app_src\components\audio\effect_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3773DDEB-ED70-483B-8D2E-AED558084B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CEFAAB-4260-4109-BCF9-0F1B0CC51E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13140" yWindow="1485" windowWidth="14295" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="home" sheetId="1" r:id="rId1"/>
@@ -138,10 +138,6 @@
     <t>MSG_MUSIC_BASS_DW</t>
   </si>
   <si>
-    <t>karaoke</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>eq7</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -236,6 +232,10 @@
   </si>
   <si>
     <t>MSG_EFFECT_SYNC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Karaoke</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -632,8 +632,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -694,8 +694,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -744,19 +744,19 @@
         <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="G2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -767,19 +767,19 @@
         <v>16</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -790,19 +790,19 @@
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -813,19 +813,19 @@
         <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -836,19 +836,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -859,19 +859,19 @@
         <v>16</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -882,19 +882,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -905,19 +905,19 @@
         <v>16</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -928,19 +928,19 @@
         <v>20</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -951,19 +951,19 @@
         <v>20</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -974,19 +974,19 @@
         <v>20</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -997,19 +997,19 @@
         <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -1020,19 +1020,19 @@
         <v>20</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -1043,19 +1043,19 @@
         <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="20.25" x14ac:dyDescent="0.35">
@@ -1066,19 +1066,19 @@
         <v>20</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.25" x14ac:dyDescent="0.35">
@@ -1089,42 +1089,42 @@
         <v>20</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="E18" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="20.25" x14ac:dyDescent="0.35">
@@ -1132,22 +1132,22 @@
         <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="G19" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.35">
@@ -1155,22 +1155,22 @@
         <v>15</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20.25" x14ac:dyDescent="0.35">
@@ -1178,22 +1178,22 @@
         <v>15</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>21</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="20.25" x14ac:dyDescent="0.35">
@@ -1201,22 +1201,22 @@
         <v>15</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="20.25" x14ac:dyDescent="0.35">
@@ -1224,22 +1224,22 @@
         <v>15</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -1247,22 +1247,22 @@
         <v>15</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="20.25" x14ac:dyDescent="0.35">
@@ -1270,22 +1270,22 @@
         <v>15</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>